<commit_message>
[EVO] Arreglos multiplataforma - 3
</commit_message>
<xml_diff>
--- a/informes/informe.xlsx
+++ b/informes/informe.xlsx
@@ -10,43 +10,28 @@
     <sheet name="Hoja 1" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="5">
+  <si>
+    <t>id_pedido</t>
+  </si>
   <si>
     <t>id_cliente</t>
   </si>
   <si>
-    <t>nombre</t>
+    <t>pvp</t>
   </si>
   <si>
-    <t>dni</t>
+    <t>pvc</t>
   </si>
   <si>
-    <t>ciudad</t>
-  </si>
-  <si>
-    <t>telefonica</t>
-  </si>
-  <si>
-    <t>A2834567</t>
-  </si>
-  <si>
-    <t>madrid</t>
-  </si>
-  <si>
-    <t>Acens</t>
-  </si>
-  <si>
-    <t>A2876453</t>
-  </si>
-  <si>
-    <t>Madrid</t>
+    <t>descuento</t>
   </si>
 </sst>
 </file>
@@ -411,21 +396,22 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="true" style="0"/>
-    <col min="2" max="2" width="12.854004" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="8.140869" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="10" customWidth="true" style="0"/>
+    <col min="3" max="3" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="4" max="4" width="6.998291" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="10" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,38 +424,47 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>6</v>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>20000</v>
+      </c>
+      <c r="D2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>15000</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <autoFilter ref="A1:D1"/>
+  <autoFilter ref="A1:E1"/>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>

</xml_diff>